<commit_message>
Added link function to ExcelDriver
</commit_message>
<xml_diff>
--- a/Beton/data/testData.xlsx
+++ b/Beton/data/testData.xlsx
@@ -3,24 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\git\PerfectoCI\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\git\Beton\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="devices3" sheetId="12" r:id="rId1"/>
+    <sheet name="devices (2)" sheetId="17" r:id="rId1"/>
     <sheet name="devices" sheetId="11" r:id="rId2"/>
     <sheet name="items" sheetId="1" r:id="rId3"/>
     <sheet name="addresses" sheetId="7" r:id="rId4"/>
-    <sheet name="null" sheetId="13" r:id="rId5"/>
+    <sheet name="signIn" sheetId="14" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>Item</t>
   </si>
@@ -123,71 +123,76 @@
     <t>browserName</t>
   </si>
   <si>
-    <t>PerfectoMobile</t>
-  </si>
-  <si>
-    <t>avner</t>
-  </si>
-  <si>
     <t>iPhone-6</t>
   </si>
   <si>
     <t>mobileOS</t>
   </si>
   <si>
-    <t>US-MA-DEMO</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>$6.26</t>
   </si>
   <si>
     <t>$59.00</t>
   </si>
   <si>
+    <t>Avner</t>
+  </si>
+  <si>
+    <t>Galaxy S5 SM-G900A</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>SATeam@perfectomobile.com</t>
+  </si>
+  <si>
+    <t>SATeam123</t>
+  </si>
+  <si>
+    <t>Hi, SA!</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>avnerg@perfectomobile.com</t>
+  </si>
+  <si>
+    <t>Hi, Avner!</t>
+  </si>
+  <si>
+    <t>shshshs@aaa.com</t>
+  </si>
+  <si>
+    <t>dsdsdsd</t>
+  </si>
+  <si>
+    <t>a1001a</t>
+  </si>
+  <si>
+    <t>Hi, Sasha!</t>
+  </si>
+  <si>
+    <t>mobileOs</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>ShirNate</t>
+  </si>
+  <si>
     <t>Raj</t>
-  </si>
-  <si>
-    <t>A1A5438E</t>
-  </si>
-  <si>
-    <t>iPad Air</t>
-  </si>
-  <si>
-    <t>.*Shared</t>
-  </si>
-  <si>
-    <t>Test Parameters</t>
-  </si>
-  <si>
-    <t>testCycle</t>
-  </si>
-  <si>
-    <t>Galaxy S5</t>
-  </si>
-  <si>
-    <t>Brian</t>
-  </si>
-  <si>
-    <t>searchItemsTest, KL024-XFS1, Kolcraft Cloud Sport Lightweight Stroller, Fuchsia Pink, $49.98</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>searchItemsTest, 9780920236161, The Paper Bag Princess, $6.26</t>
-  </si>
-  <si>
-    <t>searchItemsTest, BL201, Ninja Kitchen System Pulse, $59.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -197,14 +202,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,51 +228,6 @@
         <fgColor indexed="17"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -277,26 +238,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -578,22 +533,22 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -632,57 +587,58 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="5"/>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
         <v>32</v>
       </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" t="s">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="5"/>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
       <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H4" t="s">
-        <v>35</v>
-      </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>36</v>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -696,22 +652,22 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A2" sqref="A2:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -751,13 +707,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -776,9 +732,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="16.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="38.7109375" collapsed="true"/>
-    <col min="3" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="38.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -800,7 +756,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -822,7 +778,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -841,10 +797,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="5.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="33.7109375" collapsed="true"/>
-    <col min="4" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -899,45 +855,68 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s" s="10">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" t="s" s="11">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>48</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added links to Excel
</commit_message>
<xml_diff>
--- a/Beton/data/testData.xlsx
+++ b/Beton/data/testData.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\git\Beton\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\git\Beton\Beton\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="devices (2)" sheetId="17" r:id="rId1"/>
-    <sheet name="devices" sheetId="11" r:id="rId2"/>
-    <sheet name="items" sheetId="1" r:id="rId3"/>
-    <sheet name="addresses" sheetId="7" r:id="rId4"/>
-    <sheet name="signIn" sheetId="14" r:id="rId5"/>
+    <sheet name="signIn" sheetId="18" r:id="rId1"/>
+    <sheet name="devices (2)" sheetId="17" r:id="rId2"/>
+    <sheet name="devices" sheetId="11" r:id="rId3"/>
+    <sheet name="items" sheetId="1" r:id="rId4"/>
+    <sheet name="addresses" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
   <si>
     <t>Item</t>
   </si>
@@ -530,10 +530,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="J5" sqref="E2:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,12 +715,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,13 +784,57 @@
         <v>32</v>
       </c>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -787,7 +899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -851,72 +963,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1"/>
-    <hyperlink ref="A4" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to androidCommunityPOM; utils.VisualDriverControl
</commit_message>
<xml_diff>
--- a/Beton/data/testData.xlsx
+++ b/Beton/data/testData.xlsx
@@ -3,22 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\git\Beton\Beton\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14490" windowHeight="7020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="signIn" sheetId="18" r:id="rId1"/>
-    <sheet name="devices (2)" sheetId="17" r:id="rId2"/>
-    <sheet name="devices" sheetId="11" r:id="rId3"/>
-    <sheet name="items" sheetId="1" r:id="rId4"/>
-    <sheet name="addresses" sheetId="7" r:id="rId5"/>
+    <sheet name="signIn_android" sheetId="19" r:id="rId2"/>
+    <sheet name="devices (2)" sheetId="17" r:id="rId3"/>
+    <sheet name="devices" sheetId="11" r:id="rId4"/>
+    <sheet name="items" sheetId="1" r:id="rId5"/>
+    <sheet name="addresses" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A18:L38"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>Item</t>
   </si>
@@ -187,6 +184,15 @@
   </si>
   <si>
     <t>Raj</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>brianc@perfectomobile.com</t>
+  </si>
+  <si>
+    <t>Perfecto99</t>
   </si>
 </sst>
 </file>
@@ -533,7 +539,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +549,7 @@
     <col min="3" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -565,7 +571,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -576,7 +582,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>43</v>
       </c>
@@ -597,6 +603,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -715,11 +788,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -834,7 +907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -899,9 +972,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>

</xml_diff>

<commit_message>
Added try to excel link method, to prevent deadlock.
</commit_message>
<xml_diff>
--- a/Beton/data/testData.xlsx
+++ b/Beton/data/testData.xlsx
@@ -717,7 +717,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +775,7 @@
         <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
         <v>32</v>

</xml_diff>